<commit_message>
update cbr_data, add run dfm test
</commit_message>
<xml_diff>
--- a/data/cbr_data.xlsx
+++ b/data/cbr_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Dropbox\ПК\Desktop\giga_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Dropbox\ПК\Desktop\giga_data\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F9AC0D-E95F-433D-921A-1CBEBEB75216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C423D2-8ECB-413A-9582-C069EDC35784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4020" yWindow="4020" windowWidth="21555" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -448,7 +448,7 @@
   <dimension ref="A1:G321"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>